<commit_message>
Fixing #365, #286, #355, #367
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
+++ b/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="0" windowWidth="26000" windowHeight="28340" activeTab="1"/>
+    <workbookView xWindow="8400" yWindow="40" windowWidth="25600" windowHeight="16060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="305">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -964,7 +964,13 @@
     <t>http://BrentOzar.com/go/deadlocks</t>
   </si>
   <si>
-    <t>sp_Blitz® Check ID List - v34 April 2, 2014</t>
+    <t>Plan Cache Erased Recently</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/askbrent/plan-cache-erased-recently/</t>
+  </si>
+  <si>
+    <t>sp_Blitz® Check ID List - v35 June 17, 2014</t>
   </si>
 </sst>
 </file>
@@ -2048,13 +2054,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E189"/>
+  <dimension ref="A1:E190"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B139" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2069,7 +2075,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" thickBot="1">
       <c r="A1" s="8" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1">
@@ -5222,6 +5228,23 @@
       </c>
       <c r="E189" s="6" t="s">
         <v>301</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="A190" s="4">
+        <v>125</v>
+      </c>
+      <c r="B190" s="5">
+        <v>10</v>
+      </c>
+      <c r="C190" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D190" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="E190" s="5" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Fixing #365, #286, #355, #367"
This reverts commit 636fdf81c9d0a1e55f9368ca53ddf30770666e72.
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
+++ b/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="40" windowWidth="25600" windowHeight="16060" activeTab="1"/>
+    <workbookView xWindow="1160" yWindow="0" windowWidth="26000" windowHeight="28340" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="303">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -964,13 +964,7 @@
     <t>http://BrentOzar.com/go/deadlocks</t>
   </si>
   <si>
-    <t>Plan Cache Erased Recently</t>
-  </si>
-  <si>
-    <t>http://BrentOzar.com/askbrent/plan-cache-erased-recently/</t>
-  </si>
-  <si>
-    <t>sp_Blitz® Check ID List - v35 June 17, 2014</t>
+    <t>sp_Blitz® Check ID List - v34 April 2, 2014</t>
   </si>
 </sst>
 </file>
@@ -2054,13 +2048,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E190"/>
+  <dimension ref="A1:E189"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B139" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2075,7 +2069,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" thickBot="1">
       <c r="A1" s="8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1">
@@ -5228,23 +5222,6 @@
       </c>
       <c r="E189" s="6" t="s">
         <v>301</v>
-      </c>
-    </row>
-    <row r="190" spans="1:5">
-      <c r="A190" s="4">
-        <v>125</v>
-      </c>
-      <c r="B190" s="5">
-        <v>10</v>
-      </c>
-      <c r="C190" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D190" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="E190" s="5" t="s">
-        <v>303</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#33 - output server name if CheckServerInfo = 1
Added to a row in the 250 priority section, new check id 130. Also
removed an old merge typo while I was in there.
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
+++ b/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="2400" yWindow="2600" windowWidth="25600" windowHeight="16060"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="305">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -944,9 +944,6 @@
     <t>http://BrentOzar.com/askbrent/plan-cache-erased-recently/</t>
   </si>
   <si>
-    <t>sp_Blitz® Check ID List - v35 June 17, 2014</t>
-  </si>
-  <si>
     <t>Priority Boost Enabled</t>
   </si>
   <si>
@@ -966,6 +963,12 @@
   </si>
   <si>
     <t>Dangerous Build of SQL Server</t>
+  </si>
+  <si>
+    <t>sp_Blitz® Check ID List - v36 Aug 16, 2014</t>
+  </si>
+  <si>
+    <t>Server Name</t>
   </si>
 </sst>
 </file>
@@ -1410,13 +1413,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E194"/>
+  <dimension ref="A1:E195"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B185" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B186" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A194" sqref="A194"/>
+      <selection pane="bottomRight" activeCell="A196" sqref="A196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1431,7 +1434,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" thickBot="1">
       <c r="A1" s="7" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1">
@@ -4614,10 +4617,10 @@
         <v>91</v>
       </c>
       <c r="D191" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="E191" s="5" t="s">
         <v>297</v>
-      </c>
-      <c r="E191" s="5" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -4631,10 +4634,10 @@
         <v>89</v>
       </c>
       <c r="D192" s="4" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E192" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -4648,10 +4651,10 @@
         <v>91</v>
       </c>
       <c r="D193" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E193" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -4665,10 +4668,24 @@
         <v>91</v>
       </c>
       <c r="D194" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E194" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5">
+      <c r="A195" s="3">
+        <v>130</v>
+      </c>
+      <c r="B195" s="4">
+        <v>250</v>
+      </c>
+      <c r="C195" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D195" s="4" t="s">
+        <v>304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v36 for public release
 	Changes in v36 - October 5, 2014
	 - Added non-default database configuration checks looking at
sys.databases
	   as checks 131-144. Catches things like delayed durability, forced
params.
     - Added check for long file growths from the default trace, 151.
     - Added check for serious errors in the default trace, 150.
	 - Added Hekaton memory use and transaction error checks 145-147.
	 - Added checks for database files on network shares or Azure, 148-149.
	 - Added server name row in output when @CheckServerInfo = 1.
 	 - Moved contributions to support.brentozar.com.
	 - Check 78 for stored procs with RECOMPILE now ignores sp_Blitz%.
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
+++ b/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="2600" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="sp_Blitz" sheetId="3" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="334">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -965,10 +965,97 @@
     <t>Dangerous Build of SQL Server</t>
   </si>
   <si>
-    <t>sp_Blitz® Check ID List - v36 Aug 16, 2014</t>
-  </si>
-  <si>
     <t>Server Name</t>
+  </si>
+  <si>
+    <t>sp_Blitz® Check ID List - v36 Oct 5, 2014</t>
+  </si>
+  <si>
+    <t>Non-Default Database Config</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/dbdefaults</t>
+  </si>
+  <si>
+    <t>High Memory Use for In-Memory OLTP (Hekaton)</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/hekaton</t>
+  </si>
+  <si>
+    <t>In-Memory OLTP (Hekaton) In Use</t>
+  </si>
+  <si>
+    <t>In-Memory OLTP (Hekaton)</t>
+  </si>
+  <si>
+    <t>Transaction Errors</t>
+  </si>
+  <si>
+    <t>Database Files on Network File Shares</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/nas</t>
+  </si>
+  <si>
+    <t>Database Files Stored in Azure</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/azurefiles</t>
+  </si>
+  <si>
+    <t>Errors Logged Recently in the Default Trace</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/defaulttrace</t>
+  </si>
+  <si>
+    <t>Log File Growths Slow</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/filegrowth</t>
+  </si>
+  <si>
+    <t>Supplemental Logging Enabled</t>
+  </si>
+  <si>
+    <t>Snapshot Isolation Enabled</t>
+  </si>
+  <si>
+    <t>Read Committed Snapshot Isolation Enabled</t>
+  </si>
+  <si>
+    <t>Auto Create Stats Incremental Enabled</t>
+  </si>
+  <si>
+    <t>ANSI NULL Default Enabled</t>
+  </si>
+  <si>
+    <t>Recursive Triggers Enabled</t>
+  </si>
+  <si>
+    <t>Trustworthy Enabled</t>
+  </si>
+  <si>
+    <t>Forced Parameterization Enabled</t>
+  </si>
+  <si>
+    <t>Query Store Enabled</t>
+  </si>
+  <si>
+    <t>Change Data Capture Enabled</t>
+  </si>
+  <si>
+    <t>Containment Enabled</t>
+  </si>
+  <si>
+    <t>Target Recovery Time Changed</t>
+  </si>
+  <si>
+    <t>Delayed Durability Enabled</t>
+  </si>
+  <si>
+    <t>Memory Optimized Enabled</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1142,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1063,6 +1150,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1095,7 +1186,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1112,6 +1203,10 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1413,13 +1508,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E195"/>
+  <dimension ref="A1:E216"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B186" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A196" sqref="A196"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1434,7 +1529,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" thickBot="1">
       <c r="A1" s="7" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1">
@@ -4685,7 +4780,367 @@
         <v>132</v>
       </c>
       <c r="D195" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
+      </c>
+      <c r="E195" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5">
+      <c r="A196" s="3">
+        <v>131</v>
+      </c>
+      <c r="B196" s="4">
+        <v>210</v>
+      </c>
+      <c r="C196" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D196" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="E196" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5">
+      <c r="A197" s="3">
+        <v>132</v>
+      </c>
+      <c r="B197" s="4">
+        <v>210</v>
+      </c>
+      <c r="C197" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D197" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="E197" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5">
+      <c r="A198" s="3">
+        <v>133</v>
+      </c>
+      <c r="B198" s="4">
+        <v>210</v>
+      </c>
+      <c r="C198" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D198" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="E198" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5">
+      <c r="A199" s="3">
+        <v>134</v>
+      </c>
+      <c r="B199" s="4">
+        <v>210</v>
+      </c>
+      <c r="C199" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D199" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="E199" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5">
+      <c r="A200" s="3">
+        <v>135</v>
+      </c>
+      <c r="B200" s="4">
+        <v>210</v>
+      </c>
+      <c r="C200" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D200" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="E200" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
+      <c r="A201" s="3">
+        <v>136</v>
+      </c>
+      <c r="B201" s="4">
+        <v>210</v>
+      </c>
+      <c r="C201" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D201" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E201" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5">
+      <c r="A202" s="3">
+        <v>137</v>
+      </c>
+      <c r="B202" s="4">
+        <v>210</v>
+      </c>
+      <c r="C202" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D202" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="E202" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
+      <c r="A203" s="3">
+        <v>138</v>
+      </c>
+      <c r="B203" s="4">
+        <v>210</v>
+      </c>
+      <c r="C203" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D203" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="E203" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5">
+      <c r="A204" s="3">
+        <v>139</v>
+      </c>
+      <c r="B204" s="4">
+        <v>210</v>
+      </c>
+      <c r="C204" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D204" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="E204" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5">
+      <c r="A205" s="3">
+        <v>140</v>
+      </c>
+      <c r="B205" s="4">
+        <v>210</v>
+      </c>
+      <c r="C205" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D205" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="E205" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5">
+      <c r="A206" s="3">
+        <v>141</v>
+      </c>
+      <c r="B206" s="4">
+        <v>210</v>
+      </c>
+      <c r="C206" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D206" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="E206" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5">
+      <c r="A207" s="3">
+        <v>142</v>
+      </c>
+      <c r="B207" s="4">
+        <v>210</v>
+      </c>
+      <c r="C207" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D207" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="E207" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5">
+      <c r="A208" s="3">
+        <v>143</v>
+      </c>
+      <c r="B208" s="4">
+        <v>210</v>
+      </c>
+      <c r="C208" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D208" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="E208" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5">
+      <c r="A209" s="3">
+        <v>144</v>
+      </c>
+      <c r="B209" s="4">
+        <v>210</v>
+      </c>
+      <c r="C209" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D209" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="E209" s="4" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5">
+      <c r="A210" s="3">
+        <v>145</v>
+      </c>
+      <c r="B210" s="4">
+        <v>10</v>
+      </c>
+      <c r="C210" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D210" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="E210" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5">
+      <c r="A211" s="3">
+        <v>146</v>
+      </c>
+      <c r="B211" s="4">
+        <v>200</v>
+      </c>
+      <c r="C211" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D211" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="E211" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
+      <c r="A212" s="3">
+        <v>147</v>
+      </c>
+      <c r="B212" s="4">
+        <v>100</v>
+      </c>
+      <c r="C212" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="D212" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="E212" s="5" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5">
+      <c r="A213" s="3">
+        <v>148</v>
+      </c>
+      <c r="B213" s="4">
+        <v>50</v>
+      </c>
+      <c r="C213" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D213" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="E213" s="5" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5">
+      <c r="A214" s="3">
+        <v>149</v>
+      </c>
+      <c r="B214" s="4">
+        <v>50</v>
+      </c>
+      <c r="C214" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D214" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="E214" s="5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5">
+      <c r="A215" s="3">
+        <v>150</v>
+      </c>
+      <c r="B215" s="4">
+        <v>50</v>
+      </c>
+      <c r="C215" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D215" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="E215" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5">
+      <c r="A216" s="3">
+        <v>151</v>
+      </c>
+      <c r="B216" s="4">
+        <v>50</v>
+      </c>
+      <c r="C216" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D216" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E216" s="4" t="s">
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -4730,10 +5185,15 @@
     <hyperlink ref="E192" r:id="rId35"/>
     <hyperlink ref="E193" r:id="rId36"/>
     <hyperlink ref="E194" r:id="rId37"/>
+    <hyperlink ref="E210" r:id="rId38"/>
+    <hyperlink ref="E211" r:id="rId39"/>
+    <hyperlink ref="E212" r:id="rId40"/>
+    <hyperlink ref="E213" r:id="rId41"/>
+    <hyperlink ref="E214" r:id="rId42"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId38"/>
+  <legacyDrawing r:id="rId43"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Adding wait stats checks
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
+++ b/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="338">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -968,9 +968,6 @@
     <t>Server Name</t>
   </si>
   <si>
-    <t>sp_Blitz® Check ID List - v36 Oct 5, 2014</t>
-  </si>
-  <si>
     <t>Non-Default Database Config</t>
   </si>
   <si>
@@ -1056,6 +1053,21 @@
   </si>
   <si>
     <t>Memory Optimized Enabled</t>
+  </si>
+  <si>
+    <t>sp_Blitz® Check ID List - v37 Nov 19, 2014</t>
+  </si>
+  <si>
+    <t>Wait Stats</t>
+  </si>
+  <si>
+    <t>Top Wait Stats</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/waits</t>
+  </si>
+  <si>
+    <t>No Significant Waits Detected</t>
   </si>
 </sst>
 </file>
@@ -1508,13 +1520,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E216"/>
+  <dimension ref="A1:E218"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B197" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A219" sqref="A219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1529,7 +1541,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" thickBot="1">
       <c r="A1" s="7" t="s">
-        <v>304</v>
+        <v>333</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1">
@@ -4794,13 +4806,13 @@
         <v>210</v>
       </c>
       <c r="C196" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D196" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="E196" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="D196" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="E196" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -4811,13 +4823,13 @@
         <v>210</v>
       </c>
       <c r="C197" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D197" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="E197" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="D197" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="E197" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -4828,13 +4840,13 @@
         <v>210</v>
       </c>
       <c r="C198" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D198" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="E198" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="D198" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="E198" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -4845,13 +4857,13 @@
         <v>210</v>
       </c>
       <c r="C199" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D199" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="E199" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="D199" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="E199" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -4862,13 +4874,13 @@
         <v>210</v>
       </c>
       <c r="C200" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D200" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="E200" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="D200" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="E200" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -4879,13 +4891,13 @@
         <v>210</v>
       </c>
       <c r="C201" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D201" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="E201" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="D201" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="E201" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -4896,13 +4908,13 @@
         <v>210</v>
       </c>
       <c r="C202" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D202" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E202" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="D202" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="E202" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -4913,13 +4925,13 @@
         <v>210</v>
       </c>
       <c r="C203" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D203" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="E203" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="D203" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="E203" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -4930,13 +4942,13 @@
         <v>210</v>
       </c>
       <c r="C204" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D204" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="E204" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="D204" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="E204" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -4947,13 +4959,13 @@
         <v>210</v>
       </c>
       <c r="C205" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D205" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="E205" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="D205" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="E205" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -4964,13 +4976,13 @@
         <v>210</v>
       </c>
       <c r="C206" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D206" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="E206" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="D206" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="E206" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -4981,13 +4993,13 @@
         <v>210</v>
       </c>
       <c r="C207" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D207" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="E207" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="D207" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="E207" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -4998,13 +5010,13 @@
         <v>210</v>
       </c>
       <c r="C208" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D208" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="E208" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="D208" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="E208" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -5015,13 +5027,13 @@
         <v>210</v>
       </c>
       <c r="C209" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D209" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="E209" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="D209" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="E209" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -5035,10 +5047,10 @@
         <v>92</v>
       </c>
       <c r="D210" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="E210" s="5" t="s">
         <v>307</v>
-      </c>
-      <c r="E210" s="5" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -5052,10 +5064,10 @@
         <v>92</v>
       </c>
       <c r="D211" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E211" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -5066,13 +5078,13 @@
         <v>100</v>
       </c>
       <c r="C212" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D212" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="D212" s="4" t="s">
-        <v>311</v>
-      </c>
       <c r="E212" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -5086,10 +5098,10 @@
         <v>91</v>
       </c>
       <c r="D213" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="E213" s="5" t="s">
         <v>312</v>
-      </c>
-      <c r="E213" s="5" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -5103,10 +5115,10 @@
         <v>91</v>
       </c>
       <c r="D214" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="E214" s="5" t="s">
         <v>314</v>
-      </c>
-      <c r="E214" s="5" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -5120,10 +5132,10 @@
         <v>91</v>
       </c>
       <c r="D215" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E215" s="4" t="s">
         <v>316</v>
-      </c>
-      <c r="E215" s="4" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -5137,10 +5149,44 @@
         <v>92</v>
       </c>
       <c r="D216" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="E216" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="E216" s="4" t="s">
-        <v>319</v>
+    </row>
+    <row r="217" spans="1:5">
+      <c r="A217" s="3">
+        <v>152</v>
+      </c>
+      <c r="B217" s="4">
+        <v>240</v>
+      </c>
+      <c r="C217" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="D217" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="E217" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5">
+      <c r="A218" s="3">
+        <v>153</v>
+      </c>
+      <c r="B218" s="4">
+        <v>240</v>
+      </c>
+      <c r="C218" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="D218" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="E218" s="5" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -5190,10 +5236,12 @@
     <hyperlink ref="E212" r:id="rId40"/>
     <hyperlink ref="E213" r:id="rId41"/>
     <hyperlink ref="E214" r:id="rId42"/>
+    <hyperlink ref="E217" r:id="rId43"/>
+    <hyperlink ref="E218" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId43"/>
+  <legacyDrawing r:id="rId45"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Wait fixes, check for 32-bit servers
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
+++ b/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="340">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -1068,6 +1068,12 @@
   </si>
   <si>
     <t>No Significant Waits Detected</t>
+  </si>
+  <si>
+    <t>32-bit SQL Server Installed</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/go/32bit</t>
   </si>
 </sst>
 </file>
@@ -1520,13 +1526,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E218"/>
+  <dimension ref="A1:E219"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B197" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B198" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A219" sqref="A219"/>
+      <selection pane="bottomRight" activeCell="A220" sqref="A220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5187,6 +5193,23 @@
       </c>
       <c r="E218" s="5" t="s">
         <v>336</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5">
+      <c r="A219" s="3">
+        <v>154</v>
+      </c>
+      <c r="B219" s="4">
+        <v>10</v>
+      </c>
+      <c r="C219" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D219" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="E219" s="5" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -5238,10 +5261,11 @@
     <hyperlink ref="E214" r:id="rId42"/>
     <hyperlink ref="E217" r:id="rId43"/>
     <hyperlink ref="E218" r:id="rId44"/>
+    <hyperlink ref="E219" r:id="rId45"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId45"/>
+  <legacyDrawing r:id="rId46"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added check 155 for versions >6 mos old
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
+++ b/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="343">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -1074,6 +1074,15 @@
   </si>
   <si>
     <t>http://BrentOzar.com/go/32bit</t>
+  </si>
+  <si>
+    <t>Outdated sp_Blitz</t>
+  </si>
+  <si>
+    <t>sp_Blitz is Over 6 Months Old</t>
+  </si>
+  <si>
+    <t>http://BrentOzar.com/blitz/</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1169,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1168,6 +1177,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1204,7 +1217,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1225,6 +1238,10 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1526,10 +1543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E219"/>
+  <dimension ref="A1:E220"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B198" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B212" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A220" sqref="A220"/>
@@ -5210,6 +5227,23 @@
       </c>
       <c r="E219" s="5" t="s">
         <v>339</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5">
+      <c r="A220" s="3">
+        <v>155</v>
+      </c>
+      <c r="B220" s="4">
+        <v>0</v>
+      </c>
+      <c r="C220" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="D220" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="E220" s="5" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -5262,10 +5296,11 @@
     <hyperlink ref="E217" r:id="rId43"/>
     <hyperlink ref="E218" r:id="rId44"/>
     <hyperlink ref="E219" r:id="rId45"/>
+    <hyperlink ref="E220" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId46"/>
+  <legacyDrawing r:id="rId47"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
v38 - several fixes
Added check for MS14-044, outputs rundate as 2nd to last check,
improved wait stats checks to include more details and work if server
has been up less than an hour.
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
+++ b/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="348">
   <si>
     <t>Backups Not Performed Recently</t>
   </si>
@@ -962,9 +962,6 @@
     <t>Unsupported Build of SQL Server</t>
   </si>
   <si>
-    <t>Dangerous Build of SQL Server</t>
-  </si>
-  <si>
     <t>Server Name</t>
   </si>
   <si>
@@ -1055,9 +1052,6 @@
     <t>Memory Optimized Enabled</t>
   </si>
   <si>
-    <t>sp_Blitz® Check ID List - v37 Nov 19, 2014</t>
-  </si>
-  <si>
     <t>Wait Stats</t>
   </si>
   <si>
@@ -1083,6 +1077,27 @@
   </si>
   <si>
     <t>http://BrentOzar.com/blitz/</t>
+  </si>
+  <si>
+    <t>sp_Blitz® Check ID List - v38 Nov 20, 2014</t>
+  </si>
+  <si>
+    <t>Rundate</t>
+  </si>
+  <si>
+    <t>(Current Date)</t>
+  </si>
+  <si>
+    <t>Dangerous Build of SQL Server (Corruption)</t>
+  </si>
+  <si>
+    <t>Dangerous Build of SQL Server (Security)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://sqlperformance.com/2014/06/sql-indexes/hotfix-sql-2012-rebuilds </t>
+  </si>
+  <si>
+    <t>https://technet.microsoft.com/en-us/library/security/MS14-044</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1184,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1177,6 +1192,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1217,7 +1234,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1242,6 +1259,8 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Heading 1" xfId="6" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1543,13 +1562,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E220"/>
+  <dimension ref="A1:E222"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B212" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B211" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A220" sqref="A220"/>
+      <selection pane="bottomRight" activeCell="A223" sqref="A223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1564,7 +1583,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" thickBot="1">
       <c r="A1" s="7" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1">
@@ -4798,10 +4817,10 @@
         <v>91</v>
       </c>
       <c r="D194" s="4" t="s">
-        <v>302</v>
+        <v>344</v>
       </c>
       <c r="E194" s="5" t="s">
-        <v>300</v>
+        <v>346</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -4815,7 +4834,7 @@
         <v>132</v>
       </c>
       <c r="D195" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E195" s="4" t="s">
         <v>193</v>
@@ -4829,13 +4848,13 @@
         <v>210</v>
       </c>
       <c r="C196" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D196" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="E196" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="D196" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="E196" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -4846,13 +4865,13 @@
         <v>210</v>
       </c>
       <c r="C197" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D197" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="E197" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="D197" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="E197" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -4863,13 +4882,13 @@
         <v>210</v>
       </c>
       <c r="C198" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D198" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="E198" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="D198" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="E198" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -4880,13 +4899,13 @@
         <v>210</v>
       </c>
       <c r="C199" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D199" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="E199" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="D199" s="4" t="s">
-        <v>322</v>
-      </c>
-      <c r="E199" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -4897,13 +4916,13 @@
         <v>210</v>
       </c>
       <c r="C200" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D200" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="E200" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="D200" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="E200" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -4914,13 +4933,13 @@
         <v>210</v>
       </c>
       <c r="C201" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D201" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="E201" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="D201" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="E201" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -4931,13 +4950,13 @@
         <v>210</v>
       </c>
       <c r="C202" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D202" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="E202" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="D202" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="E202" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -4948,13 +4967,13 @@
         <v>210</v>
       </c>
       <c r="C203" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D203" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="E203" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="D203" s="4" t="s">
-        <v>326</v>
-      </c>
-      <c r="E203" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -4965,13 +4984,13 @@
         <v>210</v>
       </c>
       <c r="C204" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D204" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="E204" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="D204" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="E204" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -4982,13 +5001,13 @@
         <v>210</v>
       </c>
       <c r="C205" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D205" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="E205" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="D205" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="E205" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -4999,13 +5018,13 @@
         <v>210</v>
       </c>
       <c r="C206" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D206" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="E206" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="D206" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="E206" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -5016,13 +5035,13 @@
         <v>210</v>
       </c>
       <c r="C207" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D207" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="E207" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="D207" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="E207" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -5033,13 +5052,13 @@
         <v>210</v>
       </c>
       <c r="C208" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D208" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="E208" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="D208" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="E208" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -5050,13 +5069,13 @@
         <v>210</v>
       </c>
       <c r="C209" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D209" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="E209" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="D209" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="E209" s="4" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -5070,10 +5089,10 @@
         <v>92</v>
       </c>
       <c r="D210" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="E210" s="5" t="s">
         <v>306</v>
-      </c>
-      <c r="E210" s="5" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -5087,10 +5106,10 @@
         <v>92</v>
       </c>
       <c r="D211" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E211" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -5101,13 +5120,13 @@
         <v>100</v>
       </c>
       <c r="C212" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="D212" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="D212" s="4" t="s">
-        <v>310</v>
-      </c>
       <c r="E212" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -5121,10 +5140,10 @@
         <v>91</v>
       </c>
       <c r="D213" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E213" s="5" t="s">
         <v>311</v>
-      </c>
-      <c r="E213" s="5" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -5138,10 +5157,10 @@
         <v>91</v>
       </c>
       <c r="D214" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="E214" s="5" t="s">
         <v>313</v>
-      </c>
-      <c r="E214" s="5" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -5155,10 +5174,10 @@
         <v>91</v>
       </c>
       <c r="D215" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="E215" s="4" t="s">
         <v>315</v>
-      </c>
-      <c r="E215" s="4" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -5172,10 +5191,10 @@
         <v>92</v>
       </c>
       <c r="D216" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="E216" s="4" t="s">
         <v>317</v>
-      </c>
-      <c r="E216" s="4" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="217" spans="1:5">
@@ -5186,13 +5205,13 @@
         <v>240</v>
       </c>
       <c r="C217" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="D217" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="E217" s="5" t="s">
         <v>334</v>
-      </c>
-      <c r="D217" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="E217" s="5" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -5203,13 +5222,13 @@
         <v>240</v>
       </c>
       <c r="C218" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="D218" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="E218" s="5" t="s">
         <v>334</v>
-      </c>
-      <c r="D218" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="E218" s="5" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="219" spans="1:5">
@@ -5223,10 +5242,10 @@
         <v>92</v>
       </c>
       <c r="D219" s="4" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E219" s="5" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="220" spans="1:5">
@@ -5237,13 +5256,44 @@
         <v>0</v>
       </c>
       <c r="C220" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="D220" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="E220" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="D220" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="E220" s="5" t="s">
+    </row>
+    <row r="221" spans="1:5">
+      <c r="A221" s="3">
+        <v>156</v>
+      </c>
+      <c r="B221" s="4">
+        <v>254</v>
+      </c>
+      <c r="C221" s="4" t="s">
         <v>342</v>
+      </c>
+      <c r="D221" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5">
+      <c r="A222" s="3">
+        <v>157</v>
+      </c>
+      <c r="B222" s="4">
+        <v>20</v>
+      </c>
+      <c r="C222" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D222" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="E222" s="5" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -5287,20 +5337,19 @@
     <hyperlink ref="E191" r:id="rId34"/>
     <hyperlink ref="E192" r:id="rId35"/>
     <hyperlink ref="E193" r:id="rId36"/>
-    <hyperlink ref="E194" r:id="rId37"/>
-    <hyperlink ref="E210" r:id="rId38"/>
-    <hyperlink ref="E211" r:id="rId39"/>
-    <hyperlink ref="E212" r:id="rId40"/>
-    <hyperlink ref="E213" r:id="rId41"/>
-    <hyperlink ref="E214" r:id="rId42"/>
-    <hyperlink ref="E217" r:id="rId43"/>
-    <hyperlink ref="E218" r:id="rId44"/>
-    <hyperlink ref="E219" r:id="rId45"/>
-    <hyperlink ref="E220" r:id="rId46"/>
+    <hyperlink ref="E210" r:id="rId37"/>
+    <hyperlink ref="E211" r:id="rId38"/>
+    <hyperlink ref="E212" r:id="rId39"/>
+    <hyperlink ref="E213" r:id="rId40"/>
+    <hyperlink ref="E214" r:id="rId41"/>
+    <hyperlink ref="E217" r:id="rId42"/>
+    <hyperlink ref="E218" r:id="rId43"/>
+    <hyperlink ref="E219" r:id="rId44"/>
+    <hyperlink ref="E220" r:id="rId45"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId47"/>
+  <legacyDrawing r:id="rId46"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
v39 - Official release
Not getting enough time to put more stuff into this, shipping just to
get the case sensitivity fix out there.
</commit_message>
<xml_diff>
--- a/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
+++ b/sp_Blitz/sp_Blitz®-CheckID-List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
@@ -1079,9 +1079,6 @@
     <t>http://BrentOzar.com/blitz/</t>
   </si>
   <si>
-    <t>sp_Blitz® Check ID List - v38 Nov 20, 2014</t>
-  </si>
-  <si>
     <t>Rundate</t>
   </si>
   <si>
@@ -1098,6 +1095,9 @@
   </si>
   <si>
     <t>https://technet.microsoft.com/en-us/library/security/MS14-044</t>
+  </si>
+  <si>
+    <t>sp_Blitz® Check ID List - v39 2015-02-16</t>
   </si>
 </sst>
 </file>
@@ -1565,10 +1565,10 @@
   <dimension ref="A1:E222"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B211" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="B157" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A223" sqref="A223"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1583,7 +1583,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" thickBot="1">
       <c r="A1" s="7" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickTop="1">
@@ -4817,10 +4817,10 @@
         <v>91</v>
       </c>
       <c r="D194" s="4" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E194" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -5273,10 +5273,10 @@
         <v>254</v>
       </c>
       <c r="C221" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="D221" s="4" t="s">
         <v>342</v>
-      </c>
-      <c r="D221" s="4" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -5290,10 +5290,10 @@
         <v>91</v>
       </c>
       <c r="D222" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E222" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>